<commit_message>
Rw Updates Usage Reports_26122023
Boat Enabled
InCapacity - [10] , NodeW - [-3] , BirdW - [6] , FuelW - [23]
Host - [9 + 3] .
Rw- Local(Left Running With Cost ) - [For Business/Shop/Market only]
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.5.xlsx
+++ b/Usage_S_1.0.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C869CA9-103A-45F1-AFF4-008C52D37EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E7A0B0-1F53-405B-86FE-19AB361B88D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="183">
   <si>
     <t>UnSettled</t>
   </si>
@@ -579,6 +579,12 @@
   </si>
   <si>
     <t>27/12/2023</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Rw - Lucknow</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="251">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1971,6 +1977,66 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1980,65 +2046,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2047,8 +2056,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2333,7 +2358,7 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2367,7 @@
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
@@ -2445,7 +2470,9 @@
       <c r="E4" s="140">
         <v>20</v>
       </c>
-      <c r="F4" s="164"/>
+      <c r="F4" s="251">
+        <v>20</v>
+      </c>
       <c r="G4" s="164"/>
       <c r="H4" s="9" t="s">
         <v>1</v>
@@ -2472,7 +2499,7 @@
         <v>30</v>
       </c>
       <c r="P4" s="154">
-        <v>0.4375</v>
+        <v>0.78819444444444453</v>
       </c>
       <c r="R4" s="154">
         <v>0.84375</v>
@@ -2488,7 +2515,7 @@
       <c r="E5" s="205">
         <v>10</v>
       </c>
-      <c r="F5" s="126"/>
+      <c r="F5" s="252"/>
       <c r="G5" s="126"/>
       <c r="H5" s="9" t="s">
         <v>136</v>
@@ -2526,12 +2553,12 @@
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>1010</v>
+        <v>1170</v>
       </c>
       <c r="E6" s="166">
         <v>30</v>
       </c>
-      <c r="F6" s="127"/>
+      <c r="F6" s="253"/>
       <c r="G6" s="127"/>
       <c r="H6" s="28" t="s">
         <v>147</v>
@@ -2577,7 +2604,7 @@
       <c r="E7" s="165">
         <v>10</v>
       </c>
-      <c r="F7" s="127"/>
+      <c r="F7" s="253"/>
       <c r="G7" s="127"/>
       <c r="H7" s="9" t="s">
         <v>9</v>
@@ -2604,7 +2631,7 @@
         <v>90</v>
       </c>
       <c r="P7" s="154">
-        <v>0.4375</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>130</v>
@@ -2620,7 +2647,7 @@
       <c r="E8" s="215">
         <v>50</v>
       </c>
-      <c r="F8" s="217"/>
+      <c r="F8" s="254"/>
       <c r="G8" s="190"/>
       <c r="H8" s="9" t="s">
         <v>72</v>
@@ -2662,10 +2689,12 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6-C2</f>
-        <v>8010</v>
+        <v>8170</v>
       </c>
       <c r="E9" s="216"/>
-      <c r="F9" s="218"/>
+      <c r="F9" s="165">
+        <v>20</v>
+      </c>
       <c r="G9" s="191"/>
       <c r="H9" s="9" t="s">
         <v>71</v>
@@ -2690,7 +2719,7 @@
         <v>64</v>
       </c>
       <c r="P9" s="154">
-        <v>0.4375</v>
+        <v>0.78819444444444453</v>
       </c>
       <c r="R9" s="154">
         <v>0.79861111111111116</v>
@@ -2703,7 +2732,9 @@
       <c r="E10" s="205">
         <v>10</v>
       </c>
-      <c r="F10" s="177"/>
+      <c r="F10" s="165">
+        <v>10</v>
+      </c>
       <c r="G10" s="177"/>
       <c r="H10" s="9" t="s">
         <v>81</v>
@@ -2730,7 +2761,7 @@
         <v>66</v>
       </c>
       <c r="P10" s="154">
-        <v>0.4375</v>
+        <v>0.78819444444444453</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>126</v>
@@ -2753,7 +2784,9 @@
       <c r="E11" s="205">
         <v>10</v>
       </c>
-      <c r="F11" s="184"/>
+      <c r="F11" s="255">
+        <v>100</v>
+      </c>
       <c r="G11" s="184"/>
       <c r="H11" s="41" t="s">
         <v>128</v>
@@ -2780,7 +2813,7 @@
         <v>161</v>
       </c>
       <c r="P11" s="154">
-        <v>0.4375</v>
+        <v>0.78819444444444453</v>
       </c>
       <c r="R11" s="154">
         <v>0.84375</v>
@@ -2793,7 +2826,9 @@
       <c r="E12" s="165">
         <v>10</v>
       </c>
-      <c r="F12" s="164"/>
+      <c r="F12" s="251">
+        <v>10</v>
+      </c>
       <c r="G12" s="164"/>
       <c r="H12" s="9" t="s">
         <v>175</v>
@@ -2811,16 +2846,16 @@
         <v>152</v>
       </c>
       <c r="M12" s="187" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="N12" s="194" t="s">
         <v>123</v>
       </c>
       <c r="O12" s="188" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
       <c r="P12" s="154">
-        <v>0.4375</v>
+        <v>0.78819444444444453</v>
       </c>
       <c r="Q12" s="24"/>
       <c r="R12" s="154">
@@ -2836,7 +2871,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>8010</v>
+        <v>8170</v>
       </c>
       <c r="H13" s="28"/>
       <c r="J13" s="119"/>
@@ -2855,7 +2890,7 @@
       <c r="G14" s="189"/>
       <c r="H14" s="9">
         <f>SUM(E4:G12)</f>
-        <v>150</v>
+        <v>310</v>
       </c>
       <c r="J14" s="119"/>
       <c r="K14" s="119"/>
@@ -2873,7 +2908,7 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="20"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="20"/>
       <c r="J15" s="119"/>
       <c r="K15" s="197"/>
@@ -2886,7 +2921,7 @@
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="24"/>
-      <c r="F16" s="20"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="20"/>
       <c r="J16" s="119"/>
       <c r="K16" s="119"/>
@@ -2895,7 +2930,7 @@
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="24"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="20"/>
       <c r="J17" s="119"/>
       <c r="K17" s="119"/>
@@ -2912,7 +2947,7 @@
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="20"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="20"/>
       <c r="J18" s="119"/>
       <c r="K18" s="119"/>
@@ -2924,7 +2959,7 @@
       <c r="L19" s="206"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="P17:P18"/>
     <mergeCell ref="Q17:Q18"/>
@@ -2935,7 +2970,6 @@
     <mergeCell ref="Q13:Q15"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="E2:G2"/>
   </mergeCells>
@@ -2945,10 +2979,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,18 +3006,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="240" t="s">
+      <c r="E1" s="224" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="241"/>
+      <c r="F1" s="225"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="240" t="s">
+      <c r="H1" s="224" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="242"/>
-      <c r="J1" s="241"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="225"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -3028,26 +3062,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="243">
+      <c r="K2" s="230">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="245">
+      <c r="L2" s="232">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="230">
+      <c r="M2" s="234">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J44)</f>
-        <v>7970</v>
+        <f>SUM(E2:J45)</f>
+        <v>8130</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="229"/>
+      <c r="B3" s="228"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -3062,13 +3096,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="244"/>
-      <c r="L3" s="246"/>
-      <c r="M3" s="231"/>
+      <c r="K3" s="231"/>
+      <c r="L3" s="233"/>
+      <c r="M3" s="235"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="228"/>
+      <c r="B4" s="229"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -3083,9 +3117,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="244"/>
-      <c r="L4" s="246"/>
-      <c r="M4" s="231"/>
+      <c r="K4" s="231"/>
+      <c r="L4" s="233"/>
+      <c r="M4" s="235"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -3167,7 +3201,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="232">
+      <c r="B7" s="236">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -3184,22 +3218,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="234">
+      <c r="K7" s="238">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="236">
+      <c r="L7" s="240">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="238">
+      <c r="M7" s="242">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="233"/>
+      <c r="B8" s="237"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -3220,9 +3254,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="235"/>
-      <c r="L8" s="237"/>
-      <c r="M8" s="239"/>
+      <c r="K8" s="239"/>
+      <c r="L8" s="241"/>
+      <c r="M8" s="243"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -3302,7 +3336,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="232">
+      <c r="B11" s="236">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -3329,7 +3363,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="233"/>
+      <c r="B12" s="237"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -3386,7 +3420,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="232">
+      <c r="B14" s="236">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -3409,7 +3443,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="233"/>
+      <c r="B15" s="237"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3464,7 +3498,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="229"/>
+      <c r="B17" s="228"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3511,7 +3545,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="228"/>
+      <c r="B19" s="229"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3571,7 +3605,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="225">
+      <c r="B21" s="245">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3599,7 +3633,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="226"/>
+      <c r="B22" s="246"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -3739,7 +3773,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="224"/>
+      <c r="B27" s="244"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -4070,7 +4104,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="224"/>
+      <c r="B40" s="244"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -4125,7 +4159,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="224"/>
+      <c r="B42" s="244"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -4172,10 +4206,10 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="130">
+      <c r="B44" s="211">
         <v>26</v>
       </c>
-      <c r="C44" s="18"/>
+      <c r="C44" s="142"/>
       <c r="D44" s="18">
         <v>150</v>
       </c>
@@ -4197,13 +4231,41 @@
       <c r="L44" s="18"/>
       <c r="M44" s="18"/>
     </row>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="257"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="256">
+        <v>100</v>
+      </c>
+      <c r="H45" s="256">
+        <v>20</v>
+      </c>
+      <c r="I45" s="256">
+        <v>20</v>
+      </c>
+      <c r="J45" s="256">
+        <v>20</v>
+      </c>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+  <mergeCells count="25">
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="M2:M4"/>
@@ -4213,16 +4275,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8845,7 +8902,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="250"/>
+      <c r="AX33" s="247"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -8881,7 +8938,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="250"/>
+      <c r="BN33" s="247"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10228,7 +10285,7 @@
     </row>
     <row r="45" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="250"/>
+      <c r="C45" s="247"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -10733,14 +10790,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="202"/>
       <c r="AP51" s="203"/>
-      <c r="AQ51" s="247"/>
+      <c r="AQ51" s="248"/>
       <c r="AR51" s="202"/>
       <c r="AS51" s="204"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="248"/>
-      <c r="AV51" s="249"/>
+      <c r="AU51" s="249"/>
+      <c r="AV51" s="250"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -10748,6 +10805,22 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -10763,22 +10836,6 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Updates Usage Report_27122023
Boat Enabled
InCapacity - [0] , NodeW - [-3] , BirdW - [6] , FuelW - [12]
Host - [9 + 3] .
Rw- Local(Left Running With Cost ) - [For Business/Shop/Market only] - []
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.5.xlsx
+++ b/Usage_S_1.0.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C591A4-BEDA-4892-98B2-66497E71188C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607E5CB6-965F-4594-8987-0DF343CA6B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1445,7 +1445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1951,6 +1951,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1997,7 +2000,64 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2009,120 +2069,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2406,7 +2369,7 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,15 +2405,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="216">
+      <c r="C2" s="217">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="224" t="s">
+      <c r="E2" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="225"/>
-      <c r="G2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="227"/>
       <c r="H2" s="26" t="s">
         <v>43</v>
       </c>
@@ -2496,19 +2459,19 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="215" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="217"/>
+      <c r="C3" s="218"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="215"/>
+      <c r="A4" s="216"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -2551,7 +2514,7 @@
         <v>0.84375</v>
       </c>
       <c r="T4" s="24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2594,12 +2557,12 @@
         <v>0.84375</v>
       </c>
       <c r="T5" s="24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>1260</v>
+        <v>1350</v>
       </c>
       <c r="E6" s="166">
         <v>10</v>
@@ -2637,7 +2600,7 @@
         <v>0.85555555555555562</v>
       </c>
       <c r="T6" s="24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2648,7 +2611,9 @@
         <v>0</v>
       </c>
       <c r="E7" s="165"/>
-      <c r="F7" s="208"/>
+      <c r="F7" s="208">
+        <v>10</v>
+      </c>
       <c r="G7" s="127"/>
       <c r="H7" s="9" t="s">
         <v>9</v>
@@ -2675,7 +2640,7 @@
         <v>90</v>
       </c>
       <c r="P7" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.8125</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>130</v>
@@ -2684,11 +2649,11 @@
         <v>0.85555555555555562</v>
       </c>
       <c r="T7" s="24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="220">
+      <c r="E8" s="221">
         <v>25</v>
       </c>
       <c r="F8" s="209"/>
@@ -2699,7 +2664,7 @@
       <c r="I8" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="222" t="s">
+      <c r="J8" s="223" t="s">
         <v>105</v>
       </c>
       <c r="K8" s="83" t="s">
@@ -2724,7 +2689,7 @@
         <v>0.85555555555555562</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2733,9 +2698,9 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6-C2</f>
-        <v>8260</v>
-      </c>
-      <c r="E9" s="221"/>
+        <v>8350</v>
+      </c>
+      <c r="E9" s="222"/>
       <c r="F9" s="165"/>
       <c r="G9" s="191"/>
       <c r="H9" s="9" t="s">
@@ -2744,7 +2709,7 @@
       <c r="I9" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="223"/>
+      <c r="J9" s="224"/>
       <c r="K9" s="182" t="s">
         <v>163</v>
       </c>
@@ -2767,14 +2732,16 @@
         <v>0.79861111111111116</v>
       </c>
       <c r="T9" s="24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="271">
+      <c r="E10" s="211">
         <v>10</v>
       </c>
-      <c r="F10" s="165"/>
+      <c r="F10" s="165">
+        <v>70</v>
+      </c>
       <c r="G10" s="177"/>
       <c r="H10" s="9" t="s">
         <v>81</v>
@@ -2801,7 +2768,7 @@
         <v>66</v>
       </c>
       <c r="P10" s="154">
-        <v>0.54999999999999993</v>
+        <v>0.8125</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>126</v>
@@ -2819,9 +2786,9 @@
       </c>
       <c r="B11" s="8">
         <f>B9-B13</f>
-        <v>90</v>
-      </c>
-      <c r="E11" s="271">
+        <v>0</v>
+      </c>
+      <c r="E11" s="211">
         <v>10</v>
       </c>
       <c r="F11" s="210"/>
@@ -2862,7 +2829,9 @@
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="165"/>
-      <c r="F12" s="206"/>
+      <c r="F12" s="206">
+        <v>10</v>
+      </c>
       <c r="G12" s="164"/>
       <c r="H12" s="9" t="s">
         <v>175</v>
@@ -2889,14 +2858,14 @@
         <v>181</v>
       </c>
       <c r="P12" s="154">
-        <v>0.78819444444444453</v>
+        <v>0.8125</v>
       </c>
       <c r="Q12" s="24"/>
       <c r="R12" s="154">
         <v>0.84375</v>
       </c>
       <c r="T12" s="24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2905,32 +2874,32 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>8170</v>
+        <v>8350</v>
       </c>
       <c r="H13" s="28"/>
       <c r="J13" s="119"/>
       <c r="K13" s="119"/>
-      <c r="L13" s="211"/>
-      <c r="P13" s="212"/>
-      <c r="Q13" s="213"/>
+      <c r="L13" s="212"/>
+      <c r="P13" s="213"/>
+      <c r="Q13" s="214"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="218" t="s">
+      <c r="E14" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="219"/>
+      <c r="F14" s="220"/>
       <c r="G14" s="189"/>
       <c r="H14" s="9">
         <f>SUM(E4:G12)</f>
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="J14" s="119"/>
       <c r="K14" s="119"/>
-      <c r="L14" s="211"/>
-      <c r="P14" s="212"/>
-      <c r="Q14" s="213"/>
+      <c r="L14" s="212"/>
+      <c r="P14" s="213"/>
+      <c r="Q14" s="214"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2946,10 +2915,10 @@
       <c r="G15" s="20"/>
       <c r="J15" s="119"/>
       <c r="K15" s="197"/>
-      <c r="L15" s="211"/>
+      <c r="L15" s="212"/>
       <c r="M15" s="119"/>
-      <c r="P15" s="212"/>
-      <c r="Q15" s="213"/>
+      <c r="P15" s="213"/>
+      <c r="Q15" s="214"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C16" s="25"/>
@@ -2968,8 +2937,8 @@
       <c r="G17" s="20"/>
       <c r="J17" s="119"/>
       <c r="K17" s="119"/>
-      <c r="P17" s="212"/>
-      <c r="Q17" s="213"/>
+      <c r="P17" s="213"/>
+      <c r="Q17" s="214"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2985,12 +2954,12 @@
       <c r="G18" s="20"/>
       <c r="J18" s="119"/>
       <c r="K18" s="119"/>
-      <c r="L18" s="211"/>
-      <c r="P18" s="212"/>
-      <c r="Q18" s="213"/>
+      <c r="L18" s="212"/>
+      <c r="P18" s="213"/>
+      <c r="Q18" s="214"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L19" s="211"/>
+      <c r="L19" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3013,10 +2982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3040,18 +3009,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="244" t="s">
+      <c r="E1" s="228" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="245"/>
+      <c r="F1" s="229"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="244" t="s">
+      <c r="H1" s="228" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="246"/>
-      <c r="J1" s="245"/>
+      <c r="I1" s="230"/>
+      <c r="J1" s="229"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -3096,26 +3065,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="247">
+      <c r="K2" s="234">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="249">
+      <c r="L2" s="236">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="234">
+      <c r="M2" s="238">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J45)</f>
-        <v>8130</v>
+        <f>SUM(E2:J47)</f>
+        <v>8310</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="233"/>
+      <c r="B3" s="232"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -3130,13 +3099,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="248"/>
-      <c r="L3" s="250"/>
-      <c r="M3" s="235"/>
+      <c r="K3" s="235"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="239"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="232"/>
+      <c r="B4" s="233"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -3151,9 +3120,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="248"/>
-      <c r="L4" s="250"/>
-      <c r="M4" s="235"/>
+      <c r="K4" s="235"/>
+      <c r="L4" s="237"/>
+      <c r="M4" s="239"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -3235,7 +3204,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="236">
+      <c r="B7" s="240">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -3252,22 +3221,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="238">
+      <c r="K7" s="242">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="240">
+      <c r="L7" s="244">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="242">
+      <c r="M7" s="246">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="237"/>
+      <c r="B8" s="241"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -3288,9 +3257,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="239"/>
-      <c r="L8" s="241"/>
-      <c r="M8" s="243"/>
+      <c r="K8" s="243"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="247"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -3370,7 +3339,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="236">
+      <c r="B11" s="240">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -3397,7 +3366,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="237"/>
+      <c r="B12" s="241"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -3454,7 +3423,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="236">
+      <c r="B14" s="240">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -3477,7 +3446,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="237"/>
+      <c r="B15" s="241"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3532,7 +3501,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="233"/>
+      <c r="B17" s="232"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3579,7 +3548,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="232"/>
+      <c r="B19" s="233"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3639,7 +3608,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="229">
+      <c r="B21" s="249">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3667,7 +3636,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="230"/>
+      <c r="B22" s="250"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -3719,7 +3688,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="216">
+      <c r="B24" s="217">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -3748,7 +3717,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="217"/>
+      <c r="B25" s="218"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -3776,7 +3745,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="216">
+      <c r="B26" s="217">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -3807,7 +3776,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="228"/>
+      <c r="B27" s="248"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -3838,7 +3807,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="216">
+      <c r="B28" s="217">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -3860,7 +3829,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="217"/>
+      <c r="B29" s="218"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -3886,7 +3855,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="216">
+      <c r="B30" s="217">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -3909,7 +3878,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="217"/>
+      <c r="B31" s="218"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -3936,7 +3905,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="216">
+      <c r="B32" s="217">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -3958,7 +3927,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="217"/>
+      <c r="B33" s="218"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -4011,7 +3980,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="216">
+      <c r="B35" s="217">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -4038,7 +4007,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="217"/>
+      <c r="B36" s="218"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -4060,7 +4029,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="216">
+      <c r="B37" s="217">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -4093,7 +4062,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="217"/>
+      <c r="B38" s="218"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -4111,7 +4080,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="216">
+      <c r="B39" s="217">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -4138,7 +4107,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="228"/>
+      <c r="B40" s="248"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -4166,7 +4135,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="216">
+      <c r="B41" s="217">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -4193,7 +4162,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="228"/>
+      <c r="B42" s="248"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -4211,7 +4180,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="217"/>
+      <c r="B43" s="218"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -4240,7 +4209,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="216">
+      <c r="B44" s="217">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -4266,8 +4235,8 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="227"/>
-      <c r="C45" s="18"/>
+      <c r="B45" s="218"/>
+      <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -4291,34 +4260,59 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="130">
+      <c r="B46" s="217">
         <v>27</v>
       </c>
-      <c r="C46" s="18"/>
+      <c r="C46" s="142"/>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="272">
+      <c r="F46" s="18">
         <v>50</v>
       </c>
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
-      <c r="I46" s="272">
+      <c r="I46" s="18">
         <v>20</v>
       </c>
-      <c r="J46" s="272">
+      <c r="J46" s="18">
         <v>20</v>
       </c>
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
       <c r="M46" s="18"/>
     </row>
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="218"/>
+      <c r="C47" s="161"/>
+      <c r="D47" s="159"/>
+      <c r="E47" s="159"/>
+      <c r="F47" s="159"/>
+      <c r="G47" s="257">
+        <v>70</v>
+      </c>
+      <c r="H47" s="159"/>
+      <c r="I47" s="257">
+        <v>20</v>
+      </c>
+      <c r="J47" s="159"/>
+      <c r="K47" s="159"/>
+      <c r="L47" s="159"/>
+      <c r="M47" s="159"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+  <mergeCells count="26">
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="M2:M4"/>
@@ -4328,17 +4322,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7545,10 +7533,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="218" t="s">
+      <c r="AG24" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="219"/>
+      <c r="AH24" s="220"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -7568,10 +7556,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="218" t="s">
+      <c r="AZ24" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="219"/>
+      <c r="BA24" s="220"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -7591,10 +7579,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="218" t="s">
+      <c r="BR24" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="219"/>
+      <c r="BS24" s="220"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -7617,10 +7605,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="224" t="s">
+      <c r="B26" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="226"/>
+      <c r="C26" s="227"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -7657,10 +7645,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="224" t="s">
+      <c r="R26" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="226"/>
+      <c r="S26" s="227"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -7697,10 +7685,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="224" t="s">
+      <c r="AG26" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="226"/>
+      <c r="AH26" s="227"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -7737,10 +7725,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="224" t="s">
+      <c r="AW26" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="226"/>
+      <c r="AX26" s="227"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -7777,10 +7765,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="224" t="s">
+      <c r="BM26" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="226"/>
+      <c r="BN26" s="227"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8774,7 +8762,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="251">
+      <c r="AX32" s="254">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -8812,7 +8800,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="251">
+      <c r="BN32" s="254">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -8961,7 +8949,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="252"/>
+      <c r="AX33" s="255"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -8997,7 +8985,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="252"/>
+      <c r="BN33" s="255"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -9148,7 +9136,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="253"/>
+      <c r="AX34" s="256"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -9186,7 +9174,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="253"/>
+      <c r="BN34" s="256"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -9417,10 +9405,10 @@
       </c>
     </row>
     <row r="36" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="218" t="s">
+      <c r="B36" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="219"/>
+      <c r="C36" s="220"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -9438,10 +9426,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="218" t="s">
+      <c r="R36" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="219"/>
+      <c r="S36" s="220"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -9459,10 +9447,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="218" t="s">
+      <c r="AG36" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="219"/>
+      <c r="AH36" s="220"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -9480,10 +9468,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="218" t="s">
+      <c r="AW36" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="219"/>
+      <c r="AX36" s="220"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -9501,10 +9489,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="218" t="s">
+      <c r="BM36" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="219"/>
+      <c r="BN36" s="220"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -9524,10 +9512,10 @@
     </row>
     <row r="37" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="224" t="s">
+      <c r="B38" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="226"/>
+      <c r="C38" s="227"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -9567,10 +9555,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="224" t="s">
+      <c r="S38" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="226"/>
+      <c r="T38" s="227"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -9610,11 +9598,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="224" t="s">
+      <c r="AJ38" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="225"/>
-      <c r="AL38" s="226"/>
+      <c r="AK38" s="226"/>
+      <c r="AL38" s="227"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -9659,11 +9647,11 @@
         <f ca="1">TODAY()</f>
         <v>45287</v>
       </c>
-      <c r="BD38" s="224" t="s">
+      <c r="BD38" s="225" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="225"/>
-      <c r="BF38" s="226"/>
+      <c r="BE38" s="226"/>
+      <c r="BF38" s="227"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -9745,20 +9733,17 @@
       <c r="AY39" s="24"/>
       <c r="AZ39" s="49"/>
       <c r="BD39" s="136"/>
-      <c r="BE39" s="257"/>
-      <c r="BF39" s="258"/>
-      <c r="BG39" s="259"/>
-      <c r="BH39" s="260"/>
-      <c r="BI39" s="261"/>
-      <c r="BJ39" s="261"/>
-      <c r="BK39" s="259"/>
-      <c r="BL39" s="259"/>
-      <c r="BM39" s="262"/>
-      <c r="BN39" s="258"/>
-      <c r="BO39" s="263"/>
-      <c r="BP39" s="257"/>
-      <c r="BQ39" s="257"/>
-      <c r="BR39" s="257"/>
+      <c r="BE39" s="1"/>
+      <c r="BF39" s="2"/>
+      <c r="BH39" s="25"/>
+      <c r="BI39" s="117"/>
+      <c r="BJ39" s="117"/>
+      <c r="BM39" s="192"/>
+      <c r="BN39" s="2"/>
+      <c r="BO39" s="152"/>
+      <c r="BP39" s="1"/>
+      <c r="BQ39" s="1"/>
+      <c r="BR39" s="1"/>
       <c r="BS39" s="46"/>
     </row>
     <row r="40" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9920,14 +9905,14 @@
       <c r="BN40" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="BO40" s="264">
+      <c r="BO40" s="154">
         <v>0.78819444444444453</v>
       </c>
-      <c r="BP40" s="257"/>
-      <c r="BQ40" s="264">
+      <c r="BP40" s="1"/>
+      <c r="BQ40" s="154">
         <v>0.84375</v>
       </c>
-      <c r="BR40" s="257"/>
+      <c r="BR40" s="1"/>
       <c r="BS40" s="46" t="s">
         <v>180</v>
       </c>
@@ -10089,14 +10074,14 @@
       <c r="BN41" s="198" t="s">
         <v>86</v>
       </c>
-      <c r="BO41" s="264">
+      <c r="BO41" s="154">
         <v>0.4375</v>
       </c>
-      <c r="BP41" s="257"/>
-      <c r="BQ41" s="264">
+      <c r="BP41" s="1"/>
+      <c r="BQ41" s="154">
         <v>0.84375</v>
       </c>
-      <c r="BR41" s="257"/>
+      <c r="BR41" s="1"/>
       <c r="BS41" s="46" t="s">
         <v>168</v>
       </c>
@@ -10230,7 +10215,7 @@
       </c>
       <c r="BE42" s="208"/>
       <c r="BF42" s="127"/>
-      <c r="BG42" s="265" t="s">
+      <c r="BG42" s="28" t="s">
         <v>147</v>
       </c>
       <c r="BH42" s="120" t="s">
@@ -10254,14 +10239,14 @@
       <c r="BN42" s="176" t="s">
         <v>69</v>
       </c>
-      <c r="BO42" s="264">
+      <c r="BO42" s="154">
         <v>0.4375</v>
       </c>
-      <c r="BP42" s="257"/>
-      <c r="BQ42" s="264">
+      <c r="BP42" s="1"/>
+      <c r="BQ42" s="154">
         <v>0.85555555555555562</v>
       </c>
-      <c r="BR42" s="257"/>
+      <c r="BR42" s="1"/>
       <c r="BS42" s="46" t="s">
         <v>168</v>
       </c>
@@ -10427,23 +10412,23 @@
       <c r="BN43" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="BO43" s="264">
+      <c r="BO43" s="154">
         <v>0.79166666666666663</v>
       </c>
-      <c r="BP43" s="257" t="s">
+      <c r="BP43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="BQ43" s="264">
+      <c r="BQ43" s="154">
         <v>0.85555555555555562</v>
       </c>
-      <c r="BR43" s="257"/>
+      <c r="BR43" s="1"/>
       <c r="BS43" s="46" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="44" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="251">
+      <c r="C44" s="254">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -10481,10 +10466,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="220">
+      <c r="S44" s="221">
         <v>25</v>
       </c>
-      <c r="T44" s="251">
+      <c r="T44" s="254">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -10493,7 +10478,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="222" t="s">
+      <c r="W44" s="223" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -10522,10 +10507,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="220">
+      <c r="AJ44" s="221">
         <v>50</v>
       </c>
-      <c r="AK44" s="251">
+      <c r="AK44" s="254">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -10535,7 +10520,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="222" t="s">
+      <c r="AO44" s="223" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -10565,7 +10550,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="220">
+      <c r="BD44" s="221">
         <v>50</v>
       </c>
       <c r="BE44" s="209"/>
@@ -10576,7 +10561,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="222" t="s">
+      <c r="BI44" s="223" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -10594,21 +10579,21 @@
       <c r="BN44" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="BO44" s="264">
+      <c r="BO44" s="154">
         <v>0.4375</v>
       </c>
-      <c r="BP44" s="257"/>
-      <c r="BQ44" s="264">
+      <c r="BP44" s="1"/>
+      <c r="BQ44" s="154">
         <v>0.85555555555555562</v>
       </c>
-      <c r="BR44" s="257"/>
+      <c r="BR44" s="1"/>
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="45" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="252"/>
+      <c r="C45" s="255"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -10642,15 +10627,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="221"/>
-      <c r="T45" s="253"/>
+      <c r="S45" s="222"/>
+      <c r="T45" s="256"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="223"/>
+      <c r="W45" s="224"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -10677,8 +10662,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="221"/>
-      <c r="AK45" s="253"/>
+      <c r="AJ45" s="222"/>
+      <c r="AK45" s="256"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -10686,7 +10671,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="223"/>
+      <c r="AO45" s="224"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -10714,7 +10699,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="221"/>
+      <c r="BD45" s="222"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -10725,7 +10710,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="223"/>
+      <c r="BI45" s="224"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -10741,21 +10726,21 @@
       <c r="BN45" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="BO45" s="264">
+      <c r="BO45" s="154">
         <v>0.78819444444444453</v>
       </c>
-      <c r="BP45" s="257"/>
-      <c r="BQ45" s="264">
+      <c r="BP45" s="1"/>
+      <c r="BQ45" s="154">
         <v>0.79861111111111116</v>
       </c>
-      <c r="BR45" s="257"/>
+      <c r="BR45" s="1"/>
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="46" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="253"/>
+      <c r="C46" s="256"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -10912,16 +10897,16 @@
       <c r="BN46" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="BO46" s="264">
+      <c r="BO46" s="154">
         <v>0.78819444444444453</v>
       </c>
-      <c r="BP46" s="257" t="s">
+      <c r="BP46" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="BQ46" s="264">
+      <c r="BQ46" s="154">
         <v>0.84375</v>
       </c>
-      <c r="BR46" s="257"/>
+      <c r="BR46" s="1"/>
       <c r="BS46" s="46" t="s">
         <v>168</v>
       </c>
@@ -11085,23 +11070,23 @@
       <c r="BN47" s="199" t="s">
         <v>161</v>
       </c>
-      <c r="BO47" s="264">
+      <c r="BO47" s="154">
         <v>0.78819444444444453</v>
       </c>
-      <c r="BP47" s="257"/>
-      <c r="BQ47" s="264">
+      <c r="BP47" s="1"/>
+      <c r="BQ47" s="154">
         <v>0.84375</v>
       </c>
-      <c r="BR47" s="257"/>
+      <c r="BR47" s="1"/>
       <c r="BS47" s="46" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="48" spans="2:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="218" t="s">
+      <c r="B48" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="219"/>
+      <c r="C48" s="220"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -11120,10 +11105,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="218" t="s">
+      <c r="S48" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="219"/>
+      <c r="T48" s="220"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -11216,14 +11201,14 @@
       <c r="BN48" s="188" t="s">
         <v>181</v>
       </c>
-      <c r="BO48" s="264">
+      <c r="BO48" s="154">
         <v>0.78819444444444453</v>
       </c>
-      <c r="BP48" s="266"/>
-      <c r="BQ48" s="264">
+      <c r="BP48" s="24"/>
+      <c r="BQ48" s="154">
         <v>0.84375</v>
       </c>
-      <c r="BR48" s="257"/>
+      <c r="BR48" s="1"/>
       <c r="BS48" s="46" t="s">
         <v>168</v>
       </c>
@@ -11236,37 +11221,36 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="211"/>
+      <c r="AQ49" s="212"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="212"/>
-      <c r="AV49" s="213"/>
+      <c r="AU49" s="213"/>
+      <c r="AV49" s="214"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
       <c r="AZ49" s="49"/>
       <c r="BD49" s="136"/>
-      <c r="BE49" s="257"/>
-      <c r="BF49" s="258"/>
-      <c r="BG49" s="265"/>
-      <c r="BH49" s="260"/>
-      <c r="BI49" s="267"/>
-      <c r="BJ49" s="267"/>
-      <c r="BK49" s="268"/>
-      <c r="BL49" s="259"/>
-      <c r="BM49" s="262"/>
-      <c r="BN49" s="258"/>
-      <c r="BO49" s="269"/>
-      <c r="BP49" s="270"/>
-      <c r="BQ49" s="257"/>
-      <c r="BR49" s="257"/>
+      <c r="BE49" s="1"/>
+      <c r="BF49" s="2"/>
+      <c r="BG49" s="28"/>
+      <c r="BH49" s="25"/>
+      <c r="BI49" s="119"/>
+      <c r="BJ49" s="119"/>
+      <c r="BK49" s="212"/>
+      <c r="BM49" s="192"/>
+      <c r="BN49" s="2"/>
+      <c r="BO49" s="213"/>
+      <c r="BP49" s="214"/>
+      <c r="BQ49" s="1"/>
+      <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
     </row>
     <row r="50" spans="36:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="218" t="s">
+      <c r="AJ50" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="219"/>
+      <c r="AK50" s="220"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -11277,35 +11261,34 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="211"/>
+      <c r="AQ50" s="212"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="212"/>
-      <c r="AV50" s="213"/>
+      <c r="AU50" s="213"/>
+      <c r="AV50" s="214"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="218" t="s">
+      <c r="BD50" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="219"/>
+      <c r="BE50" s="220"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
         <v>310</v>
       </c>
-      <c r="BH50" s="260"/>
-      <c r="BI50" s="267"/>
-      <c r="BJ50" s="267"/>
-      <c r="BK50" s="268"/>
-      <c r="BL50" s="259"/>
-      <c r="BM50" s="262"/>
-      <c r="BN50" s="258"/>
-      <c r="BO50" s="269"/>
-      <c r="BP50" s="270"/>
-      <c r="BQ50" s="257"/>
-      <c r="BR50" s="257"/>
+      <c r="BH50" s="25"/>
+      <c r="BI50" s="119"/>
+      <c r="BJ50" s="119"/>
+      <c r="BK50" s="212"/>
+      <c r="BM50" s="192"/>
+      <c r="BN50" s="2"/>
+      <c r="BO50" s="213"/>
+      <c r="BP50" s="214"/>
+      <c r="BQ50" s="1"/>
+      <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
     </row>
     <row r="51" spans="36:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11316,14 +11299,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="202"/>
       <c r="AP51" s="203"/>
-      <c r="AQ51" s="254"/>
+      <c r="AQ51" s="252"/>
       <c r="AR51" s="202"/>
       <c r="AS51" s="204"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="255"/>
-      <c r="AV51" s="256"/>
+      <c r="AU51" s="253"/>
+      <c r="AV51" s="251"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -11335,27 +11318,36 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="202"/>
       <c r="BJ51" s="203"/>
-      <c r="BK51" s="254"/>
+      <c r="BK51" s="252"/>
       <c r="BL51" s="202"/>
       <c r="BM51" s="204"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="255"/>
-      <c r="BP51" s="256"/>
+      <c r="BO51" s="253"/>
+      <c r="BP51" s="251"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -11371,22 +11363,13 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>